<commit_message>
chore: Complete the FMEA hazard analysis for network, deployment, secured communication, security of exported data
</commit_message>
<xml_diff>
--- a/docmentation/artifacts/hazard_analysis_using_fmea.xlsx
+++ b/docmentation/artifacts/hazard_analysis_using_fmea.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asharma/Amit_Docs/University/2021_WinterSemester/SCS/PredictiveMaintainance_Project/scs_predictive_maintenance/docmentation/artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4895054-581A-F544-9DE6-C35F584F33DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7F6E53-AE47-CF41-8421-84328586B16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9C5515E3-B217-C74D-94E4-7AA4ACC219B1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" xr2:uid="{9C5515E3-B217-C74D-94E4-7AA4ACC219B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hazard Analysis (FMEA) - PM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="107">
   <si>
     <t>Item</t>
   </si>
@@ -281,6 +281,136 @@
 2. Descision making information must be highlighted in bold fonts
 3. Icons and color schemes must be supported with the textaul information.
 4. Use the screen property wisely</t>
+  </si>
+  <si>
+    <t>Network Ports</t>
+  </si>
+  <si>
+    <t>Server and client not able to communicate with each other</t>
+  </si>
+  <si>
+    <t>1. Server and client not able to communicate with each other
+2. System is not usable at all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Network ports are not available is used by another process
+2. Firewalls is blocking the port </t>
+  </si>
+  <si>
+    <t>1. System is not usable, User interface will show the network
+2. No REST API is called on the server side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Request IT to open the desired ports
+2. Make the PORT configurable via the environment variables
+3. Ask IT to whitelist the PORT in the firewall
+</t>
+  </si>
+  <si>
+    <t>Secured Communication</t>
+  </si>
+  <si>
+    <t>Communication between the server and client is not secured</t>
+  </si>
+  <si>
+    <t>1. The data can easily be hijacked or tempared over the wire.
+2. Loss of sensitive organisation data</t>
+  </si>
+  <si>
+    <t>1. The system is running on the public internet
+2. System is not using the HTTPS protocol for communication</t>
+  </si>
+  <si>
+    <t>1. The Headers of the REST calls are using HTTP headers
+2. One can access the system over the public internet</t>
+  </si>
+  <si>
+    <t>1. Use the HTTPS protocl for communication between server and client
+2. Install the system behind the VPN so only authorized people can access it</t>
+  </si>
+  <si>
+    <t>Export Information Security</t>
+  </si>
+  <si>
+    <t>The data exported out of the app is not secured and encrypted</t>
+  </si>
+  <si>
+    <t>1. The exported data can easily be read or modified by any user.
+2. The exported data can easily be mis-used</t>
+  </si>
+  <si>
+    <t>1. The sensitive data in the exported is not encrypted.
+2. Exported files can be opened in any freely available editors
+3. Files are not password protected</t>
+  </si>
+  <si>
+    <t>1. Files can easily be exported out, read in any freely avaibale editor</t>
+  </si>
+  <si>
+    <t>1. Encrypt the sensitive data while exporting the file,
+2. Make the file passowrd protected and only authorized person can open the files.
+3. Change the extension of the file so that not every editor can open and develop a small editor for the file in the application</t>
+  </si>
+  <si>
+    <t>User Interface Dashboard</t>
+  </si>
+  <si>
+    <t>Graphs are not easily understood by the operator. The Graphs represent the machine vitals.</t>
+  </si>
+  <si>
+    <t>1. Operator not able deduce the correct informaton from the graphs, as graphs representation is good for the operator</t>
+  </si>
+  <si>
+    <t>1. Operator will complain about the usage of the app.
+2. Operator might take wrong decisions</t>
+  </si>
+  <si>
+    <t>1. Graphs representation is not known to operator</t>
+  </si>
+  <si>
+    <t>1. Provide the different options to visualize the machine vitals like in tables</t>
+  </si>
+  <si>
+    <t>1. Not able to visualize any of the machine vitals in the dashboard
+2. Prediction computation for the machine is impossible</t>
+  </si>
+  <si>
+    <t>1.Machine Id entered during the machine addition is incorrect</t>
+  </si>
+  <si>
+    <t>New Machine Addition</t>
+  </si>
+  <si>
+    <t>New machine is not properly added to the system</t>
+  </si>
+  <si>
+    <t>1. Data is present is the telemetry file but can not be visualzied in the dashboard
+2. Getting no prediction classification for the machine</t>
+  </si>
+  <si>
+    <t>Deployment</t>
+  </si>
+  <si>
+    <t>System is not getting deployed in new environment</t>
+  </si>
+  <si>
+    <t>1. System is giving errors during the deployment as required packages are not getting installed</t>
+  </si>
+  <si>
+    <t>1. System is not deployed and hence can not be started in the target environment</t>
+  </si>
+  <si>
+    <t>1. No internet is available to download the desired packages</t>
+  </si>
+  <si>
+    <t>1. Ask the IT guys to make the internet available on the system before starting the deployment.
+2. Package the desired modules as part of the software package</t>
+  </si>
+  <si>
+    <t>1. Provide the operator a proper machine manually
+2. Create a REST API that will ping the all the machine connected to system to get the machine id
+3. Create a method in the server that will read the telemetry file for all unique machine id's available in the file
+4. Train the operator for using the new software</t>
   </si>
 </sst>
 </file>
@@ -650,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F387D1-A224-7343-8886-57AE1549C6D9}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -748,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="4">
-        <f>(E2*G2*I2)</f>
+        <f t="shared" ref="J2:J17" si="0">(E2*G2*I2)</f>
         <v>20</v>
       </c>
       <c r="K2" s="4" t="s">
@@ -787,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="4">
-        <f>(E3*G3*I3)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="K3" s="4" t="s">
@@ -826,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="4">
-        <f>(E4*G4*I4)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="K4" s="4" t="s">
@@ -865,7 +995,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="4">
-        <f>(E5*G5*I5)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="K5" s="4" t="s">
@@ -901,7 +1031,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="4">
-        <f>(E6*G6*I6)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -937,7 +1067,7 @@
         <v>2</v>
       </c>
       <c r="J7" s="4">
-        <f>(E7*G7*I7)</f>
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
       <c r="K7" s="4" t="s">
@@ -973,7 +1103,7 @@
         <v>7</v>
       </c>
       <c r="J8" s="4">
-        <f>(E8*G8*I8)</f>
+        <f t="shared" si="0"/>
         <v>350</v>
       </c>
       <c r="K8" s="4" t="s">
@@ -1009,7 +1139,7 @@
         <v>7</v>
       </c>
       <c r="J9" s="4">
-        <f>(E9*G9*I9)</f>
+        <f t="shared" si="0"/>
         <v>350</v>
       </c>
       <c r="K9" s="4" t="s">
@@ -1045,7 +1175,7 @@
         <v>8</v>
       </c>
       <c r="J10" s="4">
-        <f>(E10*G10*I10)</f>
+        <f t="shared" si="0"/>
         <v>400</v>
       </c>
       <c r="K10" s="4" t="s">
@@ -1081,56 +1211,227 @@
         <v>5</v>
       </c>
       <c r="J11" s="4">
-        <f>(E11*G11*I11)</f>
+        <f t="shared" si="0"/>
         <v>125</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="115" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="4">
+        <v>10</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="4">
+        <v>2</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="4">
+        <v>10</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="4">
+        <v>8</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="4">
+        <v>3</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="170" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="4">
+        <v>10</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="4">
+        <v>10</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="4">
+        <v>8</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="4">
+        <v>4</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="221" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="4">
+        <v>10</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="4">
+        <v>5</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16" s="4">
+        <v>1</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>19</v>
+      <c r="B17" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="4">
+        <v>7</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" s="4">
+        <v>3</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I17" s="4">
+        <v>2</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>